<commit_message>
Refactor file handling and update paths for integer overflow analysis; add new extraction scripts for ground truth and versioning.
</commit_message>
<xml_diff>
--- a/result/timestamp dependency (TP)/slither_extracted_0411.xlsx
+++ b/result/timestamp dependency (TP)/slither_extracted_0411.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10022</t>
+          <t>9474</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -468,12 +468,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10023</t>
+          <t>9476</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -483,12 +483,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10250</t>
+          <t>9499</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -498,12 +498,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10551</t>
+          <t>9500</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -513,12 +513,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10807</t>
+          <t>9505</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -528,315 +528,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2641</t>
+          <t>9521</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CrowdsaleExt</t>
+          <t>WaltonTokenLocker</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>292</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>295</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>6403</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>7512</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>8234</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>8596</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>9309</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>9334</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>9474</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>9476</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>9499</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>9500</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>9505</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>9521</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>WaltonTokenLocker</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>9779</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>9802</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>9803</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>9858</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>9890</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>CrowdsaleExt</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>9918</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>GENEOSSale</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>